<commit_message>
study ensembleModel post competition
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
   </bookViews>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,14 +50,25 @@
   </si>
   <si>
     <t>CV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ensembleModel</t>
+  </si>
+  <si>
+    <t>good but spent too much time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ensembleModel_gbm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,12 +85,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -97,8 +113,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -107,11 +129,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -185,6 +212,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -219,6 +247,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,14 +423,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" customWidth="1"/>
@@ -409,7 +439,7 @@
     <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -437,7 +467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -454,7 +484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -471,7 +501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -486,6 +516,37 @@
       </c>
       <c r="F5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.89562730000000002</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.93164999999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.90622999999999998</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.90011169999999996</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.92801</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.90617000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -495,12 +556,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -508,12 +570,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
study to add features post competition
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,14 +61,30 @@
   </si>
   <si>
     <t>ensembleModel_gbm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否补充newsDesk, sectionName,差不多。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addFeatureQuestion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clean newsDesk&amp;sectionName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not clean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +111,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,7 +135,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -121,6 +143,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -138,7 +166,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -212,7 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -247,7 +274,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -423,23 +449,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" customWidth="1"/>
     <col min="3" max="3" width="22.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -467,7 +494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -484,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -500,8 +527,11 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -517,8 +547,9 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -535,7 +566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -549,20 +580,57 @@
         <v>0.90617000000000003</v>
       </c>
     </row>
+    <row r="9" spans="1:7" s="4" customFormat="1">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.90542440000000002</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.92191000000000001</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.89119000000000004</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="4" customFormat="1">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.89829599999999998</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.92601</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.88880999999999999</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G4:G5"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -570,13 +638,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add features from text conpus post competition
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,14 +77,18 @@
   </si>
   <si>
     <t>not clean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addFeature</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,11 +149,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -166,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -240,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -274,6 +279,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -449,15 +455,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" customWidth="1"/>
@@ -466,7 +472,7 @@
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -494,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -511,7 +517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -527,11 +533,11 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -547,9 +553,9 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -566,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -580,38 +586,74 @@
         <v>0.90617000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0.90542440000000002</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.92191000000000001</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.89119000000000004</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0.89829599999999998</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.92601</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.88880999999999999</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>0.92893899999999996</v>
+      </c>
+      <c r="C12">
+        <v>0.92042000000000002</v>
+      </c>
+      <c r="D12">
+        <v>0.88973999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13">
+        <v>0.92547449999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.92284999999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.89653000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14">
+        <v>0.93502370000000001</v>
+      </c>
+      <c r="C14">
+        <v>0.92161999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.89295000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -624,13 +666,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -638,13 +680,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update for study post competition: add feature with emotion
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,14 +81,40 @@
   </si>
   <si>
     <t>addFeature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加1个属性，包含多个得分最高单词</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加多个属性，包含多个得分最高单词</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加了一个属性，关于问号和问词</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>补充newsDesk&amp;sectionName, 增加1个属性，包含多个得分最高单词</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emotion.csv</t>
+  </si>
+  <si>
+    <t>整段文字的emotion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="0.00000_ "/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,7 +165,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -154,6 +180,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -170,7 +208,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -244,7 +282,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,7 +316,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -455,79 +491,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.375" customWidth="1"/>
-    <col min="3" max="3" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="19.375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>0.93400119999999998</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>0.90751999999999999</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>0.89056999999999997</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>0.93349519999999997</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0.91988000000000003</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>0.88832</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>0.92962100000000003</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>0.92750999999999995</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>0.88926000000000005</v>
       </c>
       <c r="F4" t="s">
@@ -537,17 +573,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>0.91261340000000002</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>0.92298999999999998</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>0.88693999999999995</v>
       </c>
       <c r="F5" t="s">
@@ -555,105 +591,145 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="6">
         <v>0.89562730000000002</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="6">
         <v>0.93164999999999998</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="6">
         <v>0.90622999999999998</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="7">
         <v>0.90011169999999996</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="7">
         <v>0.92801</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="7">
         <v>0.90617000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="8">
         <v>0.90542440000000002</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="8">
         <v>0.92191000000000001</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="8">
         <v>0.89119000000000004</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="8">
         <v>0.89829599999999998</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="8">
         <v>0.92601</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="8">
         <v>0.88880999999999999</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>0.92893899999999996</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>0.92042000000000002</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>0.88973999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B13">
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="5">
         <v>0.92547449999999998</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>0.92284999999999995</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>0.89653000000000005</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B14">
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="5">
         <v>0.93502370000000001</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>0.92161999999999999</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>0.89295000000000002</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="5">
+        <v>0.91309689999999999</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.92390000000000005</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.89522999999999997</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.92717749999999999</v>
+      </c>
+      <c r="C17">
+        <v>0.92286999999999997</v>
+      </c>
+      <c r="D17">
+        <v>0.89654999999999996</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -666,13 +742,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -680,13 +756,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
study and update files for add features with text bag
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,17 +104,25 @@
   </si>
   <si>
     <t>整段文字的emotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text bag的方式，增加属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>headline, snippet, abstract都通过text bag方式，增加属性</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.00000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,20 +186,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -208,7 +216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -282,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -316,6 +325,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -491,244 +501,272 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="4" customWidth="1"/>
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>0.93400119999999998</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>0.90751999999999999</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>0.89056999999999997</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.93349519999999997</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.91988000000000003</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.88832</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.92962100000000003</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.92750999999999995</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.88926000000000005</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.91261340000000002</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.92298999999999998</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.88693999999999995</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.89562730000000002</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.93164999999999998</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.90622999999999998</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>0.90011169999999996</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.92801</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>0.90617000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>0.90542440000000002</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>0.92191000000000001</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>0.89119000000000004</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>0.89829599999999998</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>0.92601</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>0.88880999999999999</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>0.92893899999999996</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>0.92042000000000002</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.88973999999999998</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="4">
         <v>0.92547449999999998</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>0.92284999999999995</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0.89653000000000005</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="4">
         <v>0.93502370000000001</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.92161999999999999</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.89295000000000002</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="4">
         <v>0.91309689999999999</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>0.92390000000000005</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>0.89522999999999997</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="4">
+        <v>0.94431229999999999</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.91515000000000002</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.89575000000000005</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B17" s="4">
+        <v>0.92886159999999995</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.92737000000000003</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.89566000000000001</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B19" s="4">
         <v>0.92717749999999999</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>0.92286999999999997</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>0.89654999999999996</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F19" t="s">
         <v>22</v>
       </c>
     </row>
@@ -742,13 +780,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -756,13 +794,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update: headline+snippet+abstract whole text emotion
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,15 +103,19 @@
     <t>emotion.csv</t>
   </si>
   <si>
-    <t>整段文字的emotion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>text bag的方式，增加属性</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>headline, snippet, abstract都通过text bag方式，增加属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>headline+snippet+abstract整段文字的emotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>headline+snippet整段文字的emotion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,10 +507,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -736,7 +740,7 @@
         <v>0.89575000000000005</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -750,7 +754,7 @@
         <v>0.89566000000000001</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -767,7 +771,21 @@
         <v>0.89654999999999996</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B20" s="4">
+        <v>0.94538679999999997</v>
+      </c>
+      <c r="C20">
+        <v>0.92373000000000005</v>
+      </c>
+      <c r="D20">
+        <v>0.89822999999999997</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to study: change the unit to cal emotion; add every day news count
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,17 +116,25 @@
   </si>
   <si>
     <t>headline+snippet整段文字的emotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>headline+snippet整段文字，abstract整段文字的emotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>headline整段文字，abstract整段文字的emotion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,7 +228,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -294,7 +302,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -329,7 +336,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,15 +511,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" style="4" customWidth="1"/>
@@ -522,7 +528,7 @@
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -533,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -550,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -567,7 +573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -587,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -605,7 +611,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -622,7 +628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -636,7 +642,7 @@
         <v>0.90617000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -653,7 +659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -670,7 +676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -687,7 +693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="B13" s="4">
         <v>0.92547449999999998</v>
       </c>
@@ -701,7 +707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="B14" s="4">
         <v>0.93502370000000001</v>
       </c>
@@ -715,7 +721,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="B15" s="4">
         <v>0.91309689999999999</v>
       </c>
@@ -729,7 +735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="B16" s="4">
         <v>0.94431229999999999</v>
       </c>
@@ -743,7 +749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6">
       <c r="B17" s="4">
         <v>0.92886159999999995</v>
       </c>
@@ -757,7 +763,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -774,7 +780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6">
       <c r="B20" s="4">
         <v>0.94538679999999997</v>
       </c>
@@ -786,6 +792,34 @@
       </c>
       <c r="F20" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" s="4">
+        <v>0.94191199999999997</v>
+      </c>
+      <c r="C21">
+        <v>0.92674999999999996</v>
+      </c>
+      <c r="D21">
+        <v>0.89998</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="4">
+        <v>0.93780249999999998</v>
+      </c>
+      <c r="C22">
+        <v>0.92898999999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.89517000000000002</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -798,13 +832,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -812,13 +846,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update study file to check significant variable
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,17 +124,25 @@
   </si>
   <si>
     <t>headline整段文字，abstract整段文字的emotion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emotionSignificant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加了dayCount，并且用glm验证了significant</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,7 +236,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -302,6 +310,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -336,6 +345,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -511,15 +521,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" style="4" customWidth="1"/>
@@ -528,7 +538,7 @@
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -539,7 +549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -556,7 +566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -573,7 +583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -593,7 +603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -611,7 +621,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -628,7 +638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -642,7 +652,7 @@
         <v>0.90617000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -659,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -676,7 +686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -693,7 +703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" s="4">
         <v>0.92547449999999998</v>
       </c>
@@ -707,7 +717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <v>0.93502370000000001</v>
       </c>
@@ -721,7 +731,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B15" s="4">
         <v>0.91309689999999999</v>
       </c>
@@ -735,7 +745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B16" s="4">
         <v>0.94431229999999999</v>
       </c>
@@ -749,7 +759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B17" s="4">
         <v>0.92886159999999995</v>
       </c>
@@ -763,7 +773,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -780,7 +790,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B20" s="4">
         <v>0.94538679999999997</v>
       </c>
@@ -794,7 +804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B21" s="4">
         <v>0.94191199999999997</v>
       </c>
@@ -808,7 +818,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B22" s="4">
         <v>0.93780249999999998</v>
       </c>
@@ -820,6 +830,23 @@
       </c>
       <c r="F22" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.94631730000000003</v>
+      </c>
+      <c r="C24">
+        <v>0.93213999999999997</v>
+      </c>
+      <c r="D24">
+        <v>0.90183999999999997</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -832,13 +859,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -846,13 +873,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
study and update post competition: time list zoo
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,22 +127,33 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>emotionSignificant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>增加了dayCount，并且用glm验证了significant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>everydayCountSignificant.csv</t>
+  </si>
+  <si>
+    <t>zoo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emotion， 但是没有daycount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emotion+daycount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -310,7 +321,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -345,7 +355,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -521,15 +530,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" style="4" customWidth="1"/>
@@ -538,7 +547,7 @@
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -549,7 +558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -566,7 +575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -583,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -603,7 +612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -621,7 +630,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -638,7 +647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" s="2" customFormat="1">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -652,7 +661,7 @@
         <v>0.90617000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -669,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -686,7 +695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -703,7 +712,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="B13" s="4">
         <v>0.92547449999999998</v>
       </c>
@@ -717,7 +726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="B14" s="4">
         <v>0.93502370000000001</v>
       </c>
@@ -731,7 +740,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="B15" s="4">
         <v>0.91309689999999999</v>
       </c>
@@ -745,7 +754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="B16" s="4">
         <v>0.94431229999999999</v>
       </c>
@@ -759,7 +768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6">
       <c r="B17" s="4">
         <v>0.92886159999999995</v>
       </c>
@@ -773,7 +782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -790,7 +799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6">
       <c r="B20" s="4">
         <v>0.94538679999999997</v>
       </c>
@@ -804,7 +813,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6">
       <c r="B21" s="4">
         <v>0.94191199999999997</v>
       </c>
@@ -818,7 +827,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6">
       <c r="B22" s="4">
         <v>0.93780249999999998</v>
       </c>
@@ -832,9 +841,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" s="4">
         <v>0.94631730000000003</v>
@@ -846,7 +855,38 @@
         <v>0.90183999999999997</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.97146809999999995</v>
+      </c>
+      <c r="C27">
+        <v>0.92774000000000001</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.90649000000000002</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28" s="4">
+        <v>0.99303450000000004</v>
+      </c>
+      <c r="C28">
+        <v>0.93023</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.90966000000000002</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -859,13 +899,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -873,13 +913,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete competition study after competition end
</commit_message>
<xml_diff>
--- a/kaggleCompetition/post-study/scores.xlsx
+++ b/kaggleCompetition/post-study/scores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>本地auc</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -138,22 +138,46 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>emotion， 但是没有daycount</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>emotion+daycount</t>
+    <t>zoo， 但是没有daycount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoo(last20)+daycount, last20使用glm验证significant出来的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoo+daycount，last1/3/5/10/20/50都用了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>upper + isHoliday</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>final caretEssemble</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>final caretStack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>final model + caretEssemble组合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>final model + caretStack组合</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +188,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -204,7 +236,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -231,6 +263,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -247,7 +285,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -321,6 +359,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -355,6 +394,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -530,15 +570,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" style="4" customWidth="1"/>
@@ -547,7 +587,7 @@
     <col min="7" max="7" width="44.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -558,7 +598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -575,7 +615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -592,7 +632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -612,7 +652,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -630,7 +670,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -647,7 +687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -661,7 +701,7 @@
         <v>0.90617000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -678,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -695,7 +735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -712,7 +752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" s="4">
         <v>0.92547449999999998</v>
       </c>
@@ -726,7 +766,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B14" s="4">
         <v>0.93502370000000001</v>
       </c>
@@ -740,7 +780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B15" s="4">
         <v>0.91309689999999999</v>
       </c>
@@ -754,7 +794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B16" s="4">
         <v>0.94431229999999999</v>
       </c>
@@ -768,7 +808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B17" s="4">
         <v>0.92886159999999995</v>
       </c>
@@ -782,7 +822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -799,7 +839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B20" s="4">
         <v>0.94538679999999997</v>
       </c>
@@ -813,7 +853,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B21" s="4">
         <v>0.94191199999999997</v>
       </c>
@@ -827,7 +867,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B22" s="4">
         <v>0.93780249999999998</v>
       </c>
@@ -841,7 +881,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -858,7 +898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -875,7 +915,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B28" s="4">
         <v>0.99303450000000004</v>
       </c>
@@ -887,6 +927,68 @@
       </c>
       <c r="F28" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B29" s="4">
+        <v>0.99179969999999995</v>
+      </c>
+      <c r="C29">
+        <v>0.93113000000000001</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.91022000000000003</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="10">
+        <v>0.99501810000000002</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0.93186000000000002</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0.91218999999999995</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0.91866800000000004</v>
+      </c>
+      <c r="C32">
+        <v>0.92879</v>
+      </c>
+      <c r="D32">
+        <v>0.91354999999999997</v>
+      </c>
+      <c r="F32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0.964333</v>
+      </c>
+      <c r="C33">
+        <v>0.92278000000000004</v>
+      </c>
+      <c r="D33">
+        <v>0.90917999999999999</v>
+      </c>
+      <c r="F33" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -899,13 +1001,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -913,13 +1015,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>